<commit_message>
sotck dinámico de los combos descuenta del producto base
</commit_message>
<xml_diff>
--- a/listas/ImportarPreciosPOSCarnaveDF PUBLICO.xlsx
+++ b/listas/ImportarPreciosPOSCarnaveDF PUBLICO.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35cfd8ec92face1f/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51524EB0-82B5-42CD-81EF-AA031FAE3FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRECIOS_DE_VENTA" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PRECIOS_DE_VENTA!$A$1:$L$1000</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="0">PRECIOS_DE_VENTA!$A$2:$N$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="684">
   <si>
     <t>#PLANILLA DE FORMACIÓN DE PRECIOS PARA SISTEMA POS CARNAVE</t>
   </si>
@@ -1975,12 +1976,129 @@
   </si>
   <si>
     <t>PAPAS PRINGLES</t>
+  </si>
+  <si>
+    <t>MILANESA DE CERDO</t>
+  </si>
+  <si>
+    <t>MIX ENERGETICO</t>
+  </si>
+  <si>
+    <t>SALSA DE SOJA</t>
+  </si>
+  <si>
+    <t>PASTA DE MANI</t>
+  </si>
+  <si>
+    <t>ARROZ GALLO</t>
+  </si>
+  <si>
+    <t>ATUN AL NATURAL</t>
+  </si>
+  <si>
+    <t>ATUN EN ACEITE</t>
+  </si>
+  <si>
+    <t>MANI SALADO,SABOR,PELADO</t>
+  </si>
+  <si>
+    <t>MANI C/CASCARA</t>
+  </si>
+  <si>
+    <t>ESENCIA DE VAINILLA</t>
+  </si>
+  <si>
+    <t>ACEITE DE COCO</t>
+  </si>
+  <si>
+    <t>SALSA DE HUMO</t>
+  </si>
+  <si>
+    <t>PALITOS ZYMA</t>
+  </si>
+  <si>
+    <t>FRUTOS SECOS S/PASAS</t>
+  </si>
+  <si>
+    <t>TOSTADAS LIGTH</t>
+  </si>
+  <si>
+    <t>ALMOHADITAS RELLENAS</t>
+  </si>
+  <si>
+    <t>PASTA MULTICEREAL MAIZ</t>
+  </si>
+  <si>
+    <t>PASTA MULTICEREAL QUINOA</t>
+  </si>
+  <si>
+    <t>PASTA MULTICEREAL CHIA</t>
+  </si>
+  <si>
+    <t>PECHUGA REVENTA</t>
+  </si>
+  <si>
+    <t>ALAS REVENTA</t>
+  </si>
+  <si>
+    <t>PATA Y MUSLO REVENTA</t>
+  </si>
+  <si>
+    <t>MEDIA TARDE</t>
+  </si>
+  <si>
+    <t>LEVADURA LEVEX</t>
+  </si>
+  <si>
+    <t>PULPA DURAZNO</t>
+  </si>
+  <si>
+    <t>PULPA MELON</t>
+  </si>
+  <si>
+    <t>PULPA FRUTILLA</t>
+  </si>
+  <si>
+    <t>ACEITUNAS NEGRAS</t>
+  </si>
+  <si>
+    <t>FAJITAS DE PECHUGA</t>
+  </si>
+  <si>
+    <t>COPOZ MAIZ AZUCARADO</t>
+  </si>
+  <si>
+    <t>COPOZ MAIZ S/AZUCAR</t>
+  </si>
+  <si>
+    <t>BOLITA CHOCO</t>
+  </si>
+  <si>
+    <t>ARITOS FRUTALES</t>
+  </si>
+  <si>
+    <t>ARITOS CEREALES Y MIEL</t>
+  </si>
+  <si>
+    <t>NINA CRANBERRY</t>
+  </si>
+  <si>
+    <t>NINA BLONDIES</t>
+  </si>
+  <si>
+    <t>NINA LEMON</t>
+  </si>
+  <si>
+    <t>ETCHAR PRIVADO</t>
+  </si>
+  <si>
+    <t>POLVO DE HORNEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00&quot; &quot;%"/>
     <numFmt numFmtId="165" formatCode="0&quot; &quot;%"/>
@@ -2853,7 +2971,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3175,37 +3293,38 @@
     <xf numFmtId="4" fontId="17" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="26">
-    <cellStyle name="Accent" xfId="1"/>
-    <cellStyle name="Accent 1" xfId="2"/>
-    <cellStyle name="Accent 2" xfId="3"/>
-    <cellStyle name="Accent 3" xfId="4"/>
-    <cellStyle name="Bad" xfId="5"/>
-    <cellStyle name="Error" xfId="6"/>
-    <cellStyle name="Excel_BuiltIn_Percent" xfId="7"/>
-    <cellStyle name="Footnote" xfId="8"/>
-    <cellStyle name="Good" xfId="9"/>
-    <cellStyle name="Heading" xfId="10"/>
-    <cellStyle name="Heading 1" xfId="11"/>
-    <cellStyle name="Heading 2" xfId="12"/>
+    <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Bad" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Error" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Excel_BuiltIn_Percent" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Footnote" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Good" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Heading" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Heading 1" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Heading 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="13" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Normal 2" xfId="14"/>
-    <cellStyle name="Normal 3" xfId="15"/>
-    <cellStyle name="Normal 4" xfId="16"/>
-    <cellStyle name="Note" xfId="17"/>
+    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 3" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 4" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Note" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Porcentaje" xfId="25" builtinId="5"/>
-    <cellStyle name="Porcentaje 2" xfId="18"/>
-    <cellStyle name="Porcentaje 3" xfId="19"/>
-    <cellStyle name="Result" xfId="20"/>
-    <cellStyle name="Status" xfId="21"/>
-    <cellStyle name="Text" xfId="22"/>
-    <cellStyle name="Texto explicativo 2" xfId="23"/>
-    <cellStyle name="Warning" xfId="24"/>
+    <cellStyle name="Porcentaje 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Porcentaje 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Result" xfId="20" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Status" xfId="21" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Text" xfId="22" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Texto explicativo 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Warning" xfId="24" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3516,11 +3635,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H403" sqref="H403"/>
+    <sheetView tabSelected="1" topLeftCell="A553" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I572" sqref="I572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15.75"/>
@@ -3540,17 +3659,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="20.25">
-      <c r="A1" s="125" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
+      <c r="A1" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
       <c r="J1" s="121" t="s">
         <v>549</v>
       </c>
@@ -5515,11 +5634,11 @@
         <v>4500</v>
       </c>
       <c r="H49" s="22">
-        <v>0.33300000000000002</v>
+        <v>0.66659999999999997</v>
       </c>
       <c r="I49" s="23">
         <f t="shared" ref="I49:I60" si="6">+ROUND((G49*H49)+G49,0)</f>
-        <v>5999</v>
+        <v>7500</v>
       </c>
       <c r="J49">
         <f t="shared" si="1"/>
@@ -5531,7 +5650,7 @@
       </c>
       <c r="L49">
         <f t="shared" si="3"/>
-        <v>5999</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -6226,11 +6345,11 @@
         <v>7305.75</v>
       </c>
       <c r="H66" s="36">
-        <v>0.36859999999999998</v>
+        <v>0.27160000000000001</v>
       </c>
       <c r="I66" s="37">
         <f t="shared" si="7"/>
-        <v>9999</v>
+        <v>9290</v>
       </c>
       <c r="J66">
         <f t="shared" si="1"/>
@@ -6242,7 +6361,7 @@
       </c>
       <c r="L66">
         <f t="shared" si="3"/>
-        <v>9999</v>
+        <v>9290</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -24740,7 +24859,7 @@
     </row>
     <row r="522" spans="1:12">
       <c r="A522" s="93"/>
-      <c r="B522" s="94"/>
+      <c r="B522" s="125"/>
       <c r="C522" s="94"/>
       <c r="D522" s="95"/>
       <c r="E522" s="47"/>
@@ -25117,7 +25236,7 @@
         <v>11250</v>
       </c>
       <c r="H531" s="22">
-        <v>0.26577000000000001</v>
+        <v>0.26579999999999998</v>
       </c>
       <c r="I531" s="23">
         <f t="shared" si="78"/>
@@ -25332,11 +25451,11 @@
         <v>11880</v>
       </c>
       <c r="H536" s="22">
-        <v>0.1507</v>
+        <v>0.1187</v>
       </c>
       <c r="I536" s="23">
         <f t="shared" si="82"/>
-        <v>13670</v>
+        <v>13290</v>
       </c>
       <c r="J536">
         <f t="shared" si="76"/>
@@ -25348,7 +25467,7 @@
       </c>
       <c r="L536">
         <f t="shared" si="80"/>
-        <v>13670</v>
+        <v>13290</v>
       </c>
     </row>
     <row r="537" spans="1:12">
@@ -25461,11 +25580,11 @@
         <v>10890</v>
       </c>
       <c r="H539" s="22">
-        <v>0.2</v>
+        <v>0.1157</v>
       </c>
       <c r="I539" s="23">
         <f t="shared" si="82"/>
-        <v>13068</v>
+        <v>12150</v>
       </c>
       <c r="J539">
         <f t="shared" si="76"/>
@@ -25477,7 +25596,7 @@
       </c>
       <c r="L539">
         <f t="shared" si="80"/>
-        <v>13068</v>
+        <v>12150</v>
       </c>
     </row>
     <row r="540" spans="1:12">
@@ -25709,21 +25828,21 @@
         <v>227</v>
       </c>
       <c r="E545" s="19">
-        <v>20700</v>
+        <v>10528</v>
       </c>
       <c r="F545" s="20">
         <v>0</v>
       </c>
       <c r="G545" s="21">
         <f t="shared" si="81"/>
-        <v>20700</v>
+        <v>10528</v>
       </c>
       <c r="H545" s="22">
-        <v>0.2</v>
+        <v>0.14929999999999999</v>
       </c>
       <c r="I545" s="23">
         <f t="shared" si="82"/>
-        <v>24840</v>
+        <v>12100</v>
       </c>
       <c r="J545">
         <f t="shared" si="76"/>
@@ -25735,7 +25854,7 @@
       </c>
       <c r="L545">
         <f t="shared" si="80"/>
-        <v>24840</v>
+        <v>12100</v>
       </c>
     </row>
     <row r="546" spans="1:12">
@@ -26844,11 +26963,11 @@
         <v>11875</v>
       </c>
       <c r="H572" s="22">
-        <v>0.25</v>
+        <v>0.15110000000000001</v>
       </c>
       <c r="I572" s="23">
         <f>+ROUND((G572*H572)+G572,0)</f>
-        <v>14844</v>
+        <v>13669</v>
       </c>
       <c r="J572">
         <f t="shared" si="76"/>
@@ -26860,7 +26979,7 @@
       </c>
       <c r="L572">
         <f t="shared" si="80"/>
-        <v>14844</v>
+        <v>13669</v>
       </c>
     </row>
     <row r="573" spans="1:12">
@@ -26986,11 +27105,11 @@
         <v>6086</v>
       </c>
       <c r="H576" s="22">
-        <v>0.25</v>
+        <v>0.252</v>
       </c>
       <c r="I576" s="23">
         <f t="shared" ref="I576:I598" si="86">+ROUND((G576*H576)+G576,0)</f>
-        <v>7608</v>
+        <v>7620</v>
       </c>
       <c r="J576">
         <f t="shared" si="76"/>
@@ -27002,7 +27121,7 @@
       </c>
       <c r="L576">
         <f t="shared" si="80"/>
-        <v>7608</v>
+        <v>7620</v>
       </c>
     </row>
     <row r="577" spans="1:12">
@@ -27075,8 +27194,7 @@
         <v>0.25</v>
       </c>
       <c r="I578" s="23">
-        <f t="shared" si="86"/>
-        <v>7841</v>
+        <v>7300</v>
       </c>
       <c r="J578">
         <f t="shared" si="76"/>
@@ -27088,7 +27206,7 @@
       </c>
       <c r="L578">
         <f t="shared" si="80"/>
-        <v>7841</v>
+        <v>7300</v>
       </c>
     </row>
     <row r="579" spans="1:12">
@@ -27105,21 +27223,21 @@
         <v>227</v>
       </c>
       <c r="E579" s="19">
-        <v>6779</v>
+        <v>6273</v>
       </c>
       <c r="F579" s="20">
         <v>0</v>
       </c>
       <c r="G579" s="21">
         <f t="shared" si="85"/>
-        <v>6779</v>
+        <v>6273</v>
       </c>
       <c r="H579" s="22">
-        <v>0.25</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="I579" s="23">
         <f t="shared" si="86"/>
-        <v>8474</v>
+        <v>7299</v>
       </c>
       <c r="J579">
         <f t="shared" si="76"/>
@@ -27131,7 +27249,7 @@
       </c>
       <c r="L579">
         <f t="shared" si="80"/>
-        <v>8474</v>
+        <v>7299</v>
       </c>
     </row>
     <row r="580" spans="1:12">
@@ -27158,11 +27276,11 @@
         <v>6500</v>
       </c>
       <c r="H580" s="22">
-        <v>0.25409999999999999</v>
+        <v>0.3518</v>
       </c>
       <c r="I580" s="23">
         <f>+ROUND((G580*H580)+G580,0)</f>
-        <v>8152</v>
+        <v>8787</v>
       </c>
       <c r="J580">
         <f t="shared" si="76"/>
@@ -27174,7 +27292,7 @@
       </c>
       <c r="L580">
         <f t="shared" si="80"/>
-        <v>8152</v>
+        <v>8787</v>
       </c>
     </row>
     <row r="581" spans="1:12">
@@ -27201,11 +27319,11 @@
         <v>5292</v>
       </c>
       <c r="H581" s="22">
-        <v>0.25</v>
+        <v>0.25090000000000001</v>
       </c>
       <c r="I581" s="23">
         <f t="shared" si="86"/>
-        <v>6615</v>
+        <v>6620</v>
       </c>
       <c r="J581">
         <f t="shared" si="76"/>
@@ -27217,7 +27335,7 @@
       </c>
       <c r="L581">
         <f t="shared" si="80"/>
-        <v>6615</v>
+        <v>6620</v>
       </c>
     </row>
     <row r="582" spans="1:12">
@@ -27287,11 +27405,10 @@
         <v>6941</v>
       </c>
       <c r="H583" s="22">
-        <v>0.25</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="I583" s="23">
-        <f t="shared" si="86"/>
-        <v>8676</v>
+        <v>7899</v>
       </c>
       <c r="J583">
         <f t="shared" si="87"/>
@@ -27303,7 +27420,7 @@
       </c>
       <c r="L583">
         <f t="shared" si="80"/>
-        <v>8676</v>
+        <v>7899</v>
       </c>
     </row>
     <row r="584" spans="1:12">
@@ -27330,11 +27447,11 @@
         <v>11850</v>
       </c>
       <c r="H584" s="22">
-        <v>0.25</v>
+        <v>0.24890000000000001</v>
       </c>
       <c r="I584" s="23">
         <f t="shared" si="86"/>
-        <v>14813</v>
+        <v>14799</v>
       </c>
       <c r="J584">
         <f t="shared" si="87"/>
@@ -27346,7 +27463,7 @@
       </c>
       <c r="L584">
         <f t="shared" si="80"/>
-        <v>14813</v>
+        <v>14799</v>
       </c>
     </row>
     <row r="585" spans="1:12">
@@ -27363,21 +27480,21 @@
         <v>227</v>
       </c>
       <c r="E585" s="19">
-        <v>5800</v>
+        <v>6400</v>
       </c>
       <c r="F585" s="20">
         <v>0</v>
       </c>
       <c r="G585" s="21">
         <f t="shared" si="85"/>
-        <v>5800</v>
+        <v>6400</v>
       </c>
       <c r="H585" s="22">
-        <v>0.29310000000000003</v>
+        <v>0.29680000000000001</v>
       </c>
       <c r="I585" s="23">
         <f t="shared" si="86"/>
-        <v>7500</v>
+        <v>8300</v>
       </c>
       <c r="J585">
         <f t="shared" si="87"/>
@@ -27389,7 +27506,7 @@
       </c>
       <c r="L585">
         <f t="shared" si="80"/>
-        <v>7500</v>
+        <v>8300</v>
       </c>
     </row>
     <row r="586" spans="1:12">
@@ -27717,11 +27834,11 @@
         <v>6914</v>
       </c>
       <c r="H593" s="22">
-        <v>0.25</v>
+        <v>0.251</v>
       </c>
       <c r="I593" s="23">
         <f t="shared" si="86"/>
-        <v>8643</v>
+        <v>8649</v>
       </c>
       <c r="J593">
         <f t="shared" si="87"/>
@@ -27733,7 +27850,7 @@
       </c>
       <c r="L593">
         <f t="shared" si="89"/>
-        <v>8643</v>
+        <v>8649</v>
       </c>
     </row>
     <row r="594" spans="1:12">
@@ -27803,11 +27920,11 @@
         <v>8749</v>
       </c>
       <c r="H595" s="22">
-        <v>0.25</v>
+        <v>0.25040000000000001</v>
       </c>
       <c r="I595" s="23">
         <f t="shared" si="86"/>
-        <v>10936</v>
+        <v>10940</v>
       </c>
       <c r="J595">
         <f t="shared" si="87"/>
@@ -27819,7 +27936,7 @@
       </c>
       <c r="L595">
         <f t="shared" si="89"/>
-        <v>10936</v>
+        <v>10940</v>
       </c>
     </row>
     <row r="596" spans="1:12">
@@ -27846,11 +27963,11 @@
         <v>6913</v>
       </c>
       <c r="H596" s="22">
-        <v>0.25</v>
+        <v>0.25119999999999998</v>
       </c>
       <c r="I596" s="23">
         <f t="shared" si="86"/>
-        <v>8641</v>
+        <v>8650</v>
       </c>
       <c r="J596">
         <f t="shared" si="87"/>
@@ -27862,7 +27979,7 @@
       </c>
       <c r="L596">
         <f t="shared" si="89"/>
-        <v>8641</v>
+        <v>8650</v>
       </c>
     </row>
     <row r="597" spans="1:12">
@@ -27889,11 +28006,11 @@
         <v>6913</v>
       </c>
       <c r="H597" s="22">
-        <v>0.25</v>
+        <v>8.4699999999999998E-2</v>
       </c>
       <c r="I597" s="23">
         <f t="shared" si="86"/>
-        <v>8641</v>
+        <v>7499</v>
       </c>
       <c r="J597">
         <f t="shared" si="87"/>
@@ -27905,7 +28022,7 @@
       </c>
       <c r="L597">
         <f t="shared" si="89"/>
-        <v>8641</v>
+        <v>7499</v>
       </c>
     </row>
     <row r="598" spans="1:12">
@@ -27932,11 +28049,11 @@
         <v>6039</v>
       </c>
       <c r="H598" s="22">
-        <v>0.4</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="I598" s="23">
         <f t="shared" si="86"/>
-        <v>8455</v>
+        <v>7700</v>
       </c>
       <c r="J598">
         <f t="shared" si="87"/>
@@ -27948,7 +28065,7 @@
       </c>
       <c r="L598">
         <f t="shared" si="89"/>
-        <v>8455</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="599" spans="1:12">
@@ -28000,11 +28117,11 @@
         <v>6236</v>
       </c>
       <c r="H600" s="22">
-        <v>0.12230000000000001</v>
+        <v>0.20269999999999999</v>
       </c>
       <c r="I600" s="23">
         <f>+ROUND((G600*H600)+G600,0)</f>
-        <v>6999</v>
+        <v>7500</v>
       </c>
       <c r="J600">
         <f t="shared" si="87"/>
@@ -28016,7 +28133,7 @@
       </c>
       <c r="L600">
         <f t="shared" si="89"/>
-        <v>6999</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="601" spans="1:12">
@@ -28086,11 +28203,11 @@
         <v>7389</v>
       </c>
       <c r="H602" s="22">
-        <v>0.25</v>
+        <v>0.2505</v>
       </c>
       <c r="I602" s="23">
         <f>+ROUND((G602*H602)+G602,0)</f>
-        <v>9236</v>
+        <v>9240</v>
       </c>
       <c r="J602">
         <f t="shared" si="87"/>
@@ -28102,7 +28219,7 @@
       </c>
       <c r="L602">
         <f t="shared" si="89"/>
-        <v>9236</v>
+        <v>9240</v>
       </c>
     </row>
     <row r="603" spans="1:12" ht="16.5" customHeight="1">
@@ -28382,21 +28499,21 @@
         <v>15</v>
       </c>
       <c r="E610" s="57">
-        <v>1050</v>
+        <v>1100</v>
       </c>
       <c r="F610" s="20">
         <v>0</v>
       </c>
       <c r="G610" s="21">
         <f t="shared" si="90"/>
-        <v>1050</v>
+        <v>1100</v>
       </c>
       <c r="H610" s="22">
-        <v>0.33300000000000002</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="I610" s="23">
         <f t="shared" si="91"/>
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="J610">
         <f t="shared" si="87"/>
@@ -28408,7 +28525,7 @@
       </c>
       <c r="L610">
         <f t="shared" si="89"/>
-        <v>1400</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="611" spans="1:12">
@@ -28511,20 +28628,21 @@
         <v>15</v>
       </c>
       <c r="E613" s="57">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="F613" s="20">
         <v>0</v>
       </c>
       <c r="G613" s="21">
         <f t="shared" si="90"/>
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="H613" s="22">
-        <v>0.4</v>
+        <v>0.187</v>
       </c>
       <c r="I613" s="23">
-        <v>1800</v>
+        <f t="shared" si="91"/>
+        <v>1899</v>
       </c>
       <c r="J613">
         <f t="shared" si="87"/>
@@ -28536,7 +28654,7 @@
       </c>
       <c r="L613">
         <f t="shared" si="89"/>
-        <v>1800</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="614" spans="1:12">
@@ -28682,21 +28800,21 @@
         <v>15</v>
       </c>
       <c r="E617" s="57">
-        <v>2250</v>
+        <v>2500</v>
       </c>
       <c r="F617" s="20">
         <v>0</v>
       </c>
       <c r="G617" s="21">
         <f t="shared" si="90"/>
-        <v>2250</v>
+        <v>2500</v>
       </c>
       <c r="H617" s="22">
-        <v>0.24399999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="I617" s="23">
         <f t="shared" si="91"/>
-        <v>2799</v>
+        <v>2900</v>
       </c>
       <c r="J617">
         <f t="shared" si="87"/>
@@ -28708,7 +28826,7 @@
       </c>
       <c r="L617">
         <f t="shared" si="89"/>
-        <v>2799</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="618" spans="1:12">
@@ -30057,21 +30175,21 @@
         <v>15</v>
       </c>
       <c r="E649" s="57">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="F649" s="20">
         <v>0</v>
       </c>
       <c r="G649" s="21">
         <f t="shared" si="92"/>
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="H649" s="22">
-        <v>0.26340000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="I649" s="23">
         <f t="shared" si="93"/>
-        <v>2400</v>
+        <v>2600</v>
       </c>
       <c r="J649">
         <f t="shared" si="94"/>
@@ -30083,7 +30201,7 @@
       </c>
       <c r="L649">
         <f t="shared" si="89"/>
-        <v>2400</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="650" spans="1:12">
@@ -30960,21 +31078,21 @@
         <v>15</v>
       </c>
       <c r="E670" s="57">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="F670" s="20">
         <v>0</v>
       </c>
       <c r="G670" s="21">
         <f t="shared" si="92"/>
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="H670" s="22">
-        <v>0.4</v>
+        <v>0.1429</v>
       </c>
       <c r="I670" s="23">
         <f t="shared" si="93"/>
-        <v>4200</v>
+        <v>4000</v>
       </c>
       <c r="J670">
         <f t="shared" si="94"/>
@@ -30986,7 +31104,7 @@
       </c>
       <c r="L670">
         <f t="shared" si="96"/>
-        <v>4200</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="671" spans="1:12">
@@ -31141,11 +31259,11 @@
         <v>5000</v>
       </c>
       <c r="H674" s="22">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I674" s="23">
         <f t="shared" si="98"/>
-        <v>6500</v>
+        <v>6000</v>
       </c>
       <c r="J674">
         <f t="shared" si="94"/>
@@ -31157,7 +31275,7 @@
       </c>
       <c r="L674">
         <f t="shared" si="96"/>
-        <v>6500</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="675" spans="1:12">
@@ -31174,21 +31292,21 @@
         <v>15</v>
       </c>
       <c r="E675" s="57">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="F675" s="20">
         <v>0</v>
       </c>
       <c r="G675" s="21">
         <f t="shared" si="97"/>
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="H675" s="22">
-        <v>0.316</v>
+        <v>0.3</v>
       </c>
       <c r="I675" s="23">
         <f t="shared" si="98"/>
-        <v>2500</v>
+        <v>2600</v>
       </c>
       <c r="J675">
         <f t="shared" si="94"/>
@@ -31200,7 +31318,7 @@
       </c>
       <c r="L675">
         <f t="shared" si="96"/>
-        <v>2500</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="676" spans="1:12">
@@ -31657,11 +31775,11 @@
         <v>1359</v>
       </c>
       <c r="H686" s="22">
-        <v>0.36499999999999999</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="I686" s="23">
         <f t="shared" si="98"/>
-        <v>1855</v>
+        <v>1899</v>
       </c>
       <c r="J686">
         <f t="shared" si="94"/>
@@ -31673,7 +31791,7 @@
       </c>
       <c r="L686">
         <f t="shared" si="96"/>
-        <v>1855</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="687" spans="1:12">
@@ -31690,21 +31808,21 @@
         <v>15</v>
       </c>
       <c r="E687" s="57">
-        <v>8000</v>
+        <v>8500</v>
       </c>
       <c r="F687" s="20">
         <v>0</v>
       </c>
       <c r="G687" s="21">
         <f t="shared" si="97"/>
-        <v>8000</v>
+        <v>8500</v>
       </c>
       <c r="H687" s="22">
         <v>0.3</v>
       </c>
       <c r="I687" s="23">
         <f t="shared" si="98"/>
-        <v>10400</v>
+        <v>11050</v>
       </c>
       <c r="J687">
         <f t="shared" si="94"/>
@@ -31716,7 +31834,7 @@
       </c>
       <c r="L687">
         <f t="shared" si="96"/>
-        <v>10400</v>
+        <v>11050</v>
       </c>
     </row>
     <row r="688" spans="1:12">
@@ -31862,21 +31980,21 @@
         <v>15</v>
       </c>
       <c r="E691" s="57">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="F691" s="20">
         <v>0</v>
       </c>
       <c r="G691" s="21">
         <f t="shared" si="97"/>
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="H691" s="22">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I691" s="23">
         <f t="shared" si="98"/>
-        <v>2600</v>
+        <v>100</v>
       </c>
       <c r="J691">
         <f t="shared" si="94"/>
@@ -31888,7 +32006,7 @@
       </c>
       <c r="L691">
         <f t="shared" si="96"/>
-        <v>2600</v>
+        <v>100</v>
       </c>
     </row>
     <row r="692" spans="1:12">
@@ -32120,21 +32238,21 @@
         <v>15</v>
       </c>
       <c r="E697" s="57">
-        <v>3700</v>
+        <v>4150</v>
       </c>
       <c r="F697" s="20">
         <v>0</v>
       </c>
       <c r="G697" s="21">
         <f t="shared" si="97"/>
-        <v>3700</v>
+        <v>4150</v>
       </c>
       <c r="H697" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I697" s="23">
         <f t="shared" si="98"/>
-        <v>3700</v>
+        <v>4980</v>
       </c>
       <c r="J697">
         <f t="shared" si="94"/>
@@ -32146,12 +32264,16 @@
       </c>
       <c r="L697">
         <f t="shared" si="96"/>
-        <v>3700</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="698" spans="1:12">
-      <c r="A698" s="15"/>
-      <c r="B698" s="16"/>
+      <c r="A698" s="15">
+        <v>999</v>
+      </c>
+      <c r="B698" s="16" t="s">
+        <v>645</v>
+      </c>
       <c r="C698" s="17">
         <v>1032</v>
       </c>
@@ -32159,38 +32281,42 @@
         <v>15</v>
       </c>
       <c r="E698" s="57">
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="F698" s="20">
         <v>0</v>
       </c>
       <c r="G698" s="21">
         <f t="shared" si="97"/>
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="H698" s="22">
-        <v>0</v>
+        <v>0.55549999999999999</v>
       </c>
       <c r="I698" s="23">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="J698" t="str">
+        <v>7000</v>
+      </c>
+      <c r="J698">
         <f t="shared" si="94"/>
-        <v/>
+        <v>999</v>
       </c>
       <c r="K698" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L698" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L698">
         <f t="shared" si="96"/>
-        <v/>
+        <v>7000</v>
       </c>
     </row>
     <row r="699" spans="1:12">
-      <c r="A699" s="15"/>
-      <c r="B699" s="16"/>
+      <c r="A699" s="15">
+        <v>6091</v>
+      </c>
+      <c r="B699" s="16" t="s">
+        <v>647</v>
+      </c>
       <c r="C699" s="17">
         <v>1032</v>
       </c>
@@ -32198,38 +32324,42 @@
         <v>15</v>
       </c>
       <c r="E699" s="57">
-        <v>0</v>
+        <v>2390</v>
       </c>
       <c r="F699" s="20">
         <v>0</v>
       </c>
       <c r="G699" s="21">
         <f t="shared" si="97"/>
-        <v>0</v>
+        <v>2390</v>
       </c>
       <c r="H699" s="22">
         <v>0</v>
       </c>
       <c r="I699" s="23">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="J699" t="str">
+        <v>2390</v>
+      </c>
+      <c r="J699">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6091</v>
       </c>
       <c r="K699" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L699" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L699">
         <f t="shared" si="96"/>
-        <v/>
+        <v>2390</v>
       </c>
     </row>
     <row r="700" spans="1:12">
-      <c r="A700" s="15"/>
-      <c r="B700" s="16"/>
+      <c r="A700" s="15">
+        <v>6092</v>
+      </c>
+      <c r="B700" s="16" t="s">
+        <v>648</v>
+      </c>
       <c r="C700" s="17">
         <v>1032</v>
       </c>
@@ -32237,38 +32367,42 @@
         <v>15</v>
       </c>
       <c r="E700" s="57">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="F700" s="20">
         <v>0</v>
       </c>
       <c r="G700" s="21">
         <f t="shared" si="97"/>
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="H700" s="22">
-        <v>0</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="I700" s="23">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="J700" t="str">
+        <v>3489</v>
+      </c>
+      <c r="J700">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6092</v>
       </c>
       <c r="K700" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L700" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L700">
         <f t="shared" si="96"/>
-        <v/>
+        <v>3489</v>
       </c>
     </row>
     <row r="701" spans="1:12">
-      <c r="A701" s="15"/>
-      <c r="B701" s="16"/>
+      <c r="A701" s="15">
+        <v>6093</v>
+      </c>
+      <c r="B701" s="16" t="s">
+        <v>649</v>
+      </c>
       <c r="C701" s="17">
         <v>1032</v>
       </c>
@@ -32276,38 +32410,42 @@
         <v>15</v>
       </c>
       <c r="E701" s="57">
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="F701" s="20">
         <v>0</v>
       </c>
       <c r="G701" s="21">
         <f t="shared" si="97"/>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="H701" s="22">
-        <v>0</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="I701" s="23">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="J701" t="str">
+        <v>2600</v>
+      </c>
+      <c r="J701">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6093</v>
       </c>
       <c r="K701" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L701" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L701">
         <f t="shared" si="96"/>
-        <v/>
+        <v>2600</v>
       </c>
     </row>
     <row r="702" spans="1:12">
-      <c r="A702" s="15"/>
-      <c r="B702" s="16"/>
+      <c r="A702" s="15">
+        <v>6094</v>
+      </c>
+      <c r="B702" s="16" t="s">
+        <v>650</v>
+      </c>
       <c r="C702" s="17">
         <v>1032</v>
       </c>
@@ -32315,38 +32453,42 @@
         <v>15</v>
       </c>
       <c r="E702" s="57">
-        <v>0</v>
+        <v>2380</v>
       </c>
       <c r="F702" s="20">
         <v>0</v>
       </c>
       <c r="G702" s="21">
         <f t="shared" si="97"/>
-        <v>0</v>
+        <v>2380</v>
       </c>
       <c r="H702" s="22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I702" s="23">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="J702" t="str">
+        <v>3094</v>
+      </c>
+      <c r="J702">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6094</v>
       </c>
       <c r="K702" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L702" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L702">
         <f t="shared" si="96"/>
-        <v/>
+        <v>3094</v>
       </c>
     </row>
     <row r="703" spans="1:12">
-      <c r="A703" s="15"/>
-      <c r="B703" s="16"/>
+      <c r="A703" s="15">
+        <v>6095</v>
+      </c>
+      <c r="B703" s="16" t="s">
+        <v>651</v>
+      </c>
       <c r="C703" s="17">
         <v>1032</v>
       </c>
@@ -32354,38 +32496,42 @@
         <v>15</v>
       </c>
       <c r="E703" s="57">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F703" s="20">
         <v>0</v>
       </c>
       <c r="G703" s="21">
         <f t="shared" ref="G703:G734" si="99">E703*(1-F703)</f>
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="H703" s="22">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="I703" s="23">
         <f t="shared" ref="I703:I734" si="100">+ROUND((G703*H703)+G703,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J703" t="str">
+        <v>1755</v>
+      </c>
+      <c r="J703">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6095</v>
       </c>
       <c r="K703" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L703" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L703">
         <f t="shared" si="96"/>
-        <v/>
+        <v>1755</v>
       </c>
     </row>
     <row r="704" spans="1:12">
-      <c r="A704" s="15"/>
-      <c r="B704" s="16"/>
+      <c r="A704" s="15">
+        <v>6096</v>
+      </c>
+      <c r="B704" s="16" t="s">
+        <v>652</v>
+      </c>
       <c r="C704" s="17">
         <v>1032</v>
       </c>
@@ -32393,38 +32539,42 @@
         <v>15</v>
       </c>
       <c r="E704" s="57">
-        <v>0</v>
+        <v>6230</v>
       </c>
       <c r="F704" s="20">
         <v>0</v>
       </c>
       <c r="G704" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>6230</v>
       </c>
       <c r="H704" s="22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I704" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J704" t="str">
+        <v>8099</v>
+      </c>
+      <c r="J704">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6096</v>
       </c>
       <c r="K704" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L704" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L704">
         <f t="shared" si="96"/>
-        <v/>
+        <v>8099</v>
       </c>
     </row>
     <row r="705" spans="1:12">
-      <c r="A705" s="15"/>
-      <c r="B705" s="16"/>
+      <c r="A705" s="15">
+        <v>6097</v>
+      </c>
+      <c r="B705" s="16" t="s">
+        <v>653</v>
+      </c>
       <c r="C705" s="17">
         <v>1032</v>
       </c>
@@ -32432,38 +32582,42 @@
         <v>15</v>
       </c>
       <c r="E705" s="57">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="F705" s="20">
         <v>0</v>
       </c>
       <c r="G705" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="H705" s="22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I705" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J705" t="str">
+        <v>7800</v>
+      </c>
+      <c r="J705">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6097</v>
       </c>
       <c r="K705" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L705" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L705">
         <f t="shared" si="96"/>
-        <v/>
+        <v>7800</v>
       </c>
     </row>
     <row r="706" spans="1:12">
-      <c r="A706" s="15"/>
-      <c r="B706" s="16"/>
+      <c r="A706" s="15">
+        <v>6098</v>
+      </c>
+      <c r="B706" s="16" t="s">
+        <v>654</v>
+      </c>
       <c r="C706" s="17">
         <v>1032</v>
       </c>
@@ -32471,38 +32625,42 @@
         <v>15</v>
       </c>
       <c r="E706" s="57">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F706" s="20">
         <v>0</v>
       </c>
       <c r="G706" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="H706" s="22">
         <v>0</v>
       </c>
       <c r="I706" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J706" t="str">
+        <v>850</v>
+      </c>
+      <c r="J706">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6098</v>
       </c>
       <c r="K706" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L706" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L706">
         <f t="shared" si="96"/>
-        <v/>
+        <v>850</v>
       </c>
     </row>
     <row r="707" spans="1:12">
-      <c r="A707" s="15"/>
-      <c r="B707" s="16"/>
+      <c r="A707" s="15">
+        <v>6099</v>
+      </c>
+      <c r="B707" s="16" t="s">
+        <v>655</v>
+      </c>
       <c r="C707" s="17">
         <v>1032</v>
       </c>
@@ -32510,38 +32668,42 @@
         <v>15</v>
       </c>
       <c r="E707" s="57">
-        <v>0</v>
+        <v>3100</v>
       </c>
       <c r="F707" s="20">
         <v>0</v>
       </c>
       <c r="G707" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>3100</v>
       </c>
       <c r="H707" s="22">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="I707" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J707" t="str">
+        <v>4123</v>
+      </c>
+      <c r="J707">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6099</v>
       </c>
       <c r="K707" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L707" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L707">
         <f t="shared" si="96"/>
-        <v/>
+        <v>4123</v>
       </c>
     </row>
     <row r="708" spans="1:12">
-      <c r="A708" s="15"/>
-      <c r="B708" s="16"/>
+      <c r="A708" s="15">
+        <v>6100</v>
+      </c>
+      <c r="B708" s="16" t="s">
+        <v>656</v>
+      </c>
       <c r="C708" s="17">
         <v>1032</v>
       </c>
@@ -32549,38 +32711,42 @@
         <v>15</v>
       </c>
       <c r="E708" s="57">
-        <v>0</v>
+        <v>1550</v>
       </c>
       <c r="F708" s="20">
         <v>0</v>
       </c>
       <c r="G708" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1550</v>
       </c>
       <c r="H708" s="22">
         <v>0</v>
       </c>
       <c r="I708" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J708" t="str">
+        <v>1550</v>
+      </c>
+      <c r="J708">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6100</v>
       </c>
       <c r="K708" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L708" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L708">
         <f t="shared" si="96"/>
-        <v/>
+        <v>1550</v>
       </c>
     </row>
     <row r="709" spans="1:12">
-      <c r="A709" s="15"/>
-      <c r="B709" s="16"/>
+      <c r="A709" s="15">
+        <v>6101</v>
+      </c>
+      <c r="B709" s="16" t="s">
+        <v>657</v>
+      </c>
       <c r="C709" s="17">
         <v>1032</v>
       </c>
@@ -32588,38 +32754,42 @@
         <v>15</v>
       </c>
       <c r="E709" s="57">
-        <v>0</v>
+        <v>4390</v>
       </c>
       <c r="F709" s="20">
         <v>0</v>
       </c>
       <c r="G709" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>4390</v>
       </c>
       <c r="H709" s="22">
-        <v>0</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="I709" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J709" t="str">
+        <v>6159</v>
+      </c>
+      <c r="J709">
         <f t="shared" si="94"/>
-        <v/>
+        <v>6101</v>
       </c>
       <c r="K709" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L709" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L709">
         <f t="shared" si="96"/>
-        <v/>
+        <v>6159</v>
       </c>
     </row>
     <row r="710" spans="1:12">
-      <c r="A710" s="15"/>
-      <c r="B710" s="16"/>
+      <c r="A710" s="15">
+        <v>6102</v>
+      </c>
+      <c r="B710" s="16" t="s">
+        <v>658</v>
+      </c>
       <c r="C710" s="17">
         <v>1032</v>
       </c>
@@ -32627,38 +32797,42 @@
         <v>15</v>
       </c>
       <c r="E710" s="57">
-        <v>0</v>
+        <v>2550</v>
       </c>
       <c r="F710" s="20">
         <v>0</v>
       </c>
       <c r="G710" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>2550</v>
       </c>
       <c r="H710" s="22">
-        <v>0</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="I710" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J710" t="str">
+        <v>3300</v>
+      </c>
+      <c r="J710">
         <f t="shared" ref="J710:J773" si="101">IF(ISNUMBER(A710), IF(C710=1032, A710, "00" &amp; A710 &amp; "." &amp; C710), "")</f>
-        <v/>
+        <v>6102</v>
       </c>
       <c r="K710" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L710" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L710">
         <f t="shared" si="96"/>
-        <v/>
+        <v>3300</v>
       </c>
     </row>
     <row r="711" spans="1:12">
-      <c r="A711" s="15"/>
-      <c r="B711" s="16"/>
+      <c r="A711" s="15">
+        <v>6103</v>
+      </c>
+      <c r="B711" s="16" t="s">
+        <v>646</v>
+      </c>
       <c r="C711" s="17">
         <v>1032</v>
       </c>
@@ -32666,38 +32840,42 @@
         <v>15</v>
       </c>
       <c r="E711" s="57">
-        <v>0</v>
+        <v>1850</v>
       </c>
       <c r="F711" s="20">
         <v>0</v>
       </c>
       <c r="G711" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1850</v>
       </c>
       <c r="H711" s="22">
-        <v>0</v>
+        <v>0.35110000000000002</v>
       </c>
       <c r="I711" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J711" t="str">
+        <v>2500</v>
+      </c>
+      <c r="J711">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6103</v>
       </c>
       <c r="K711" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L711" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L711">
         <f t="shared" si="96"/>
-        <v/>
+        <v>2500</v>
       </c>
     </row>
     <row r="712" spans="1:12">
-      <c r="A712" s="15"/>
-      <c r="B712" s="16"/>
+      <c r="A712" s="15">
+        <v>6104</v>
+      </c>
+      <c r="B712" s="16" t="s">
+        <v>659</v>
+      </c>
       <c r="C712" s="17">
         <v>1032</v>
       </c>
@@ -32705,38 +32883,42 @@
         <v>15</v>
       </c>
       <c r="E712" s="57">
-        <v>0</v>
+        <v>1060</v>
       </c>
       <c r="F712" s="20">
         <v>0</v>
       </c>
       <c r="G712" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1060</v>
       </c>
       <c r="H712" s="22">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I712" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J712" t="str">
+        <v>1325</v>
+      </c>
+      <c r="J712">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6104</v>
       </c>
       <c r="K712" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L712" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L712">
         <f t="shared" si="96"/>
-        <v/>
+        <v>1325</v>
       </c>
     </row>
     <row r="713" spans="1:12">
-      <c r="A713" s="15"/>
-      <c r="B713" s="16"/>
+      <c r="A713" s="15">
+        <v>6105</v>
+      </c>
+      <c r="B713" s="16" t="s">
+        <v>660</v>
+      </c>
       <c r="C713" s="17">
         <v>1032</v>
       </c>
@@ -32744,38 +32926,42 @@
         <v>15</v>
       </c>
       <c r="E713" s="57">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="F713" s="20">
         <v>0</v>
       </c>
       <c r="G713" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="H713" s="22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I713" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J713" t="str">
+        <v>2210</v>
+      </c>
+      <c r="J713">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6105</v>
       </c>
       <c r="K713" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L713" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L713">
         <f t="shared" si="96"/>
-        <v/>
+        <v>2210</v>
       </c>
     </row>
     <row r="714" spans="1:12">
-      <c r="A714" s="15"/>
-      <c r="B714" s="16"/>
+      <c r="A714" s="15">
+        <v>6106</v>
+      </c>
+      <c r="B714" s="16" t="s">
+        <v>661</v>
+      </c>
       <c r="C714" s="17">
         <v>1032</v>
       </c>
@@ -32783,38 +32969,42 @@
         <v>15</v>
       </c>
       <c r="E714" s="57">
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="F714" s="20">
         <v>0</v>
       </c>
       <c r="G714" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="H714" s="22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I714" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J714" t="str">
+        <v>2730</v>
+      </c>
+      <c r="J714">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6106</v>
       </c>
       <c r="K714" t="str">
         <f t="shared" si="95"/>
-        <v/>
-      </c>
-      <c r="L714" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L714">
         <f t="shared" si="96"/>
-        <v/>
+        <v>2730</v>
       </c>
     </row>
     <row r="715" spans="1:12">
-      <c r="A715" s="15"/>
-      <c r="B715" s="16"/>
+      <c r="A715" s="15">
+        <v>6107</v>
+      </c>
+      <c r="B715" s="16" t="s">
+        <v>662</v>
+      </c>
       <c r="C715" s="17">
         <v>1032</v>
       </c>
@@ -32822,38 +33012,42 @@
         <v>15</v>
       </c>
       <c r="E715" s="57">
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="F715" s="20">
         <v>0</v>
       </c>
       <c r="G715" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="H715" s="22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I715" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J715" t="str">
+        <v>2730</v>
+      </c>
+      <c r="J715">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6107</v>
       </c>
       <c r="K715" t="str">
         <f t="shared" ref="K715:K778" si="102">IF(J715="","","LISTA1")</f>
-        <v/>
-      </c>
-      <c r="L715" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L715">
         <f t="shared" ref="L715:L778" si="103">IF(J715="","",I715)</f>
-        <v/>
+        <v>2730</v>
       </c>
     </row>
     <row r="716" spans="1:12">
-      <c r="A716" s="15"/>
-      <c r="B716" s="16"/>
+      <c r="A716" s="15">
+        <v>6108</v>
+      </c>
+      <c r="B716" s="16" t="s">
+        <v>663</v>
+      </c>
       <c r="C716" s="17">
         <v>1032</v>
       </c>
@@ -32861,38 +33055,42 @@
         <v>15</v>
       </c>
       <c r="E716" s="57">
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="F716" s="20">
         <v>0</v>
       </c>
       <c r="G716" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="H716" s="22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I716" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J716" t="str">
+        <v>2730</v>
+      </c>
+      <c r="J716">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6108</v>
       </c>
       <c r="K716" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L716" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L716">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2730</v>
       </c>
     </row>
     <row r="717" spans="1:12">
-      <c r="A717" s="15"/>
-      <c r="B717" s="16"/>
+      <c r="A717" s="15">
+        <v>6109</v>
+      </c>
+      <c r="B717" s="16" t="s">
+        <v>664</v>
+      </c>
       <c r="C717" s="17">
         <v>1032</v>
       </c>
@@ -32900,38 +33098,42 @@
         <v>15</v>
       </c>
       <c r="E717" s="57">
-        <v>0</v>
+        <v>6849</v>
       </c>
       <c r="F717" s="20">
         <v>0</v>
       </c>
       <c r="G717" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>6849</v>
       </c>
       <c r="H717" s="22">
-        <v>0</v>
+        <v>0.20019999999999999</v>
       </c>
       <c r="I717" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J717" t="str">
+        <v>8220</v>
+      </c>
+      <c r="J717">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6109</v>
       </c>
       <c r="K717" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L717" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L717">
         <f t="shared" si="103"/>
-        <v/>
+        <v>8220</v>
       </c>
     </row>
     <row r="718" spans="1:12">
-      <c r="A718" s="15"/>
-      <c r="B718" s="16"/>
+      <c r="A718" s="15">
+        <v>6110</v>
+      </c>
+      <c r="B718" s="16" t="s">
+        <v>665</v>
+      </c>
       <c r="C718" s="17">
         <v>1032</v>
       </c>
@@ -32939,38 +33141,42 @@
         <v>15</v>
       </c>
       <c r="E718" s="57">
-        <v>0</v>
+        <v>1876</v>
       </c>
       <c r="F718" s="20">
         <v>0</v>
       </c>
       <c r="G718" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1876</v>
       </c>
       <c r="H718" s="22">
-        <v>0</v>
+        <v>0.20419999999999999</v>
       </c>
       <c r="I718" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J718" t="str">
+        <v>2259</v>
+      </c>
+      <c r="J718">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6110</v>
       </c>
       <c r="K718" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L718" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L718">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2259</v>
       </c>
     </row>
     <row r="719" spans="1:12">
-      <c r="A719" s="15"/>
-      <c r="B719" s="16"/>
+      <c r="A719" s="15">
+        <v>6111</v>
+      </c>
+      <c r="B719" s="16" t="s">
+        <v>666</v>
+      </c>
       <c r="C719" s="17">
         <v>1032</v>
       </c>
@@ -32978,38 +33184,42 @@
         <v>15</v>
       </c>
       <c r="E719" s="57">
-        <v>0</v>
+        <v>2113</v>
       </c>
       <c r="F719" s="20">
         <v>0</v>
       </c>
       <c r="G719" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>2113</v>
       </c>
       <c r="H719" s="22">
-        <v>0</v>
+        <v>0.20680000000000001</v>
       </c>
       <c r="I719" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J719" t="str">
+        <v>2550</v>
+      </c>
+      <c r="J719">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6111</v>
       </c>
       <c r="K719" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L719" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L719">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2550</v>
       </c>
     </row>
     <row r="720" spans="1:12">
-      <c r="A720" s="15"/>
-      <c r="B720" s="16"/>
+      <c r="A720" s="15">
+        <v>6112</v>
+      </c>
+      <c r="B720" s="16" t="s">
+        <v>667</v>
+      </c>
       <c r="C720" s="17">
         <v>1032</v>
       </c>
@@ -33017,38 +33227,42 @@
         <v>15</v>
       </c>
       <c r="E720" s="57">
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="F720" s="20">
         <v>0</v>
       </c>
       <c r="G720" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="H720" s="22">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I720" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J720" t="str">
+        <v>1204</v>
+      </c>
+      <c r="J720">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6112</v>
       </c>
       <c r="K720" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L720" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L720">
         <f t="shared" si="103"/>
-        <v/>
+        <v>1204</v>
       </c>
     </row>
     <row r="721" spans="1:12">
-      <c r="A721" s="15"/>
-      <c r="B721" s="16"/>
+      <c r="A721" s="15">
+        <v>6113</v>
+      </c>
+      <c r="B721" s="16" t="s">
+        <v>668</v>
+      </c>
       <c r="C721" s="17">
         <v>1032</v>
       </c>
@@ -33056,38 +33270,42 @@
         <v>15</v>
       </c>
       <c r="E721" s="57">
-        <v>0</v>
+        <v>890</v>
       </c>
       <c r="F721" s="20">
         <v>0</v>
       </c>
       <c r="G721" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>890</v>
       </c>
       <c r="H721" s="22">
-        <v>0</v>
+        <v>0.29210000000000003</v>
       </c>
       <c r="I721" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J721" t="str">
+        <v>1150</v>
+      </c>
+      <c r="J721">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6113</v>
       </c>
       <c r="K721" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L721" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L721">
         <f t="shared" si="103"/>
-        <v/>
+        <v>1150</v>
       </c>
     </row>
     <row r="722" spans="1:12">
-      <c r="A722" s="15"/>
-      <c r="B722" s="16"/>
+      <c r="A722" s="15">
+        <v>6114</v>
+      </c>
+      <c r="B722" s="16" t="s">
+        <v>669</v>
+      </c>
       <c r="C722" s="17">
         <v>1032</v>
       </c>
@@ -33095,38 +33313,42 @@
         <v>15</v>
       </c>
       <c r="E722" s="57">
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="F722" s="20">
         <v>0</v>
       </c>
       <c r="G722" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="H722" s="22">
-        <v>0</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="I722" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J722" t="str">
+        <v>3199</v>
+      </c>
+      <c r="J722">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6114</v>
       </c>
       <c r="K722" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L722" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L722">
         <f t="shared" si="103"/>
-        <v/>
+        <v>3199</v>
       </c>
     </row>
     <row r="723" spans="1:12">
-      <c r="A723" s="15"/>
-      <c r="B723" s="16"/>
+      <c r="A723" s="15">
+        <v>6115</v>
+      </c>
+      <c r="B723" s="16" t="s">
+        <v>670</v>
+      </c>
       <c r="C723" s="17">
         <v>1032</v>
       </c>
@@ -33134,38 +33356,42 @@
         <v>15</v>
       </c>
       <c r="E723" s="57">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="F723" s="20">
         <v>0</v>
       </c>
       <c r="G723" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="H723" s="22">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I723" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J723" t="str">
+        <v>2380</v>
+      </c>
+      <c r="J723">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6115</v>
       </c>
       <c r="K723" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L723" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L723">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2380</v>
       </c>
     </row>
     <row r="724" spans="1:12">
-      <c r="A724" s="15"/>
-      <c r="B724" s="16"/>
+      <c r="A724" s="15">
+        <v>6116</v>
+      </c>
+      <c r="B724" s="16" t="s">
+        <v>671</v>
+      </c>
       <c r="C724" s="17">
         <v>1032</v>
       </c>
@@ -33173,38 +33399,42 @@
         <v>15</v>
       </c>
       <c r="E724" s="57">
-        <v>0</v>
+        <v>3170</v>
       </c>
       <c r="F724" s="20">
         <v>0</v>
       </c>
       <c r="G724" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>3170</v>
       </c>
       <c r="H724" s="22">
-        <v>0</v>
+        <v>0.3876</v>
       </c>
       <c r="I724" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J724" t="str">
+        <v>4399</v>
+      </c>
+      <c r="J724">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6116</v>
       </c>
       <c r="K724" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L724" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L724">
         <f t="shared" si="103"/>
-        <v/>
+        <v>4399</v>
       </c>
     </row>
     <row r="725" spans="1:12">
-      <c r="A725" s="15"/>
-      <c r="B725" s="16"/>
+      <c r="A725" s="15">
+        <v>6117</v>
+      </c>
+      <c r="B725" s="16" t="s">
+        <v>672</v>
+      </c>
       <c r="C725" s="17">
         <v>1032</v>
       </c>
@@ -33212,38 +33442,42 @@
         <v>15</v>
       </c>
       <c r="E725" s="57">
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="F725" s="20">
         <v>0</v>
       </c>
       <c r="G725" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="H725" s="22">
-        <v>0</v>
+        <v>0.28070000000000001</v>
       </c>
       <c r="I725" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J725" t="str">
+        <v>2600</v>
+      </c>
+      <c r="J725">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6117</v>
       </c>
       <c r="K725" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L725" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L725">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2600</v>
       </c>
     </row>
     <row r="726" spans="1:12">
-      <c r="A726" s="15"/>
-      <c r="B726" s="16"/>
+      <c r="A726" s="15">
+        <v>6118</v>
+      </c>
+      <c r="B726" s="16" t="s">
+        <v>673</v>
+      </c>
       <c r="C726" s="17">
         <v>1032</v>
       </c>
@@ -33251,38 +33485,42 @@
         <v>15</v>
       </c>
       <c r="E726" s="57">
-        <v>0</v>
+        <v>7870</v>
       </c>
       <c r="F726" s="20">
         <v>0</v>
       </c>
       <c r="G726" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>7870</v>
       </c>
       <c r="H726" s="22">
-        <v>0</v>
+        <v>0.12959999999999999</v>
       </c>
       <c r="I726" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J726" t="str">
+        <v>8890</v>
+      </c>
+      <c r="J726">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6118</v>
       </c>
       <c r="K726" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L726" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L726">
         <f t="shared" si="103"/>
-        <v/>
+        <v>8890</v>
       </c>
     </row>
     <row r="727" spans="1:12">
-      <c r="A727" s="15"/>
-      <c r="B727" s="16"/>
+      <c r="A727" s="15">
+        <v>6120</v>
+      </c>
+      <c r="B727" s="16" t="s">
+        <v>674</v>
+      </c>
       <c r="C727" s="17">
         <v>1032</v>
       </c>
@@ -33290,38 +33528,42 @@
         <v>15</v>
       </c>
       <c r="E727" s="57">
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="F727" s="20">
         <v>0</v>
       </c>
       <c r="G727" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="H727" s="22">
-        <v>0</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="I727" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J727" t="str">
+        <v>1760</v>
+      </c>
+      <c r="J727">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6120</v>
       </c>
       <c r="K727" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L727" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L727">
         <f t="shared" si="103"/>
-        <v/>
+        <v>1760</v>
       </c>
     </row>
     <row r="728" spans="1:12">
-      <c r="A728" s="15"/>
-      <c r="B728" s="16"/>
+      <c r="A728" s="15">
+        <v>6121</v>
+      </c>
+      <c r="B728" s="16" t="s">
+        <v>675</v>
+      </c>
       <c r="C728" s="17">
         <v>1032</v>
       </c>
@@ -33329,38 +33571,42 @@
         <v>15</v>
       </c>
       <c r="E728" s="57">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="F728" s="20">
         <v>0</v>
       </c>
       <c r="G728" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="H728" s="22">
-        <v>0</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="I728" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J728" t="str">
+        <v>1470</v>
+      </c>
+      <c r="J728">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6121</v>
       </c>
       <c r="K728" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L728" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L728">
         <f t="shared" si="103"/>
-        <v/>
+        <v>1470</v>
       </c>
     </row>
     <row r="729" spans="1:12">
-      <c r="A729" s="15"/>
-      <c r="B729" s="16"/>
+      <c r="A729" s="15">
+        <v>6122</v>
+      </c>
+      <c r="B729" s="16" t="s">
+        <v>676</v>
+      </c>
       <c r="C729" s="17">
         <v>1032</v>
       </c>
@@ -33368,38 +33614,42 @@
         <v>15</v>
       </c>
       <c r="E729" s="57">
-        <v>0</v>
+        <v>1050</v>
       </c>
       <c r="F729" s="20">
         <v>0</v>
       </c>
       <c r="G729" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1050</v>
       </c>
       <c r="H729" s="22">
-        <v>0</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="I729" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J729" t="str">
+        <v>1400</v>
+      </c>
+      <c r="J729">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6122</v>
       </c>
       <c r="K729" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L729" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L729">
         <f t="shared" si="103"/>
-        <v/>
+        <v>1400</v>
       </c>
     </row>
     <row r="730" spans="1:12">
-      <c r="A730" s="15"/>
-      <c r="B730" s="16"/>
+      <c r="A730" s="15">
+        <v>6123</v>
+      </c>
+      <c r="B730" s="16" t="s">
+        <v>677</v>
+      </c>
       <c r="C730" s="17">
         <v>1032</v>
       </c>
@@ -33407,38 +33657,42 @@
         <v>15</v>
       </c>
       <c r="E730" s="57">
-        <v>0</v>
+        <v>1050</v>
       </c>
       <c r="F730" s="20">
         <v>0</v>
       </c>
       <c r="G730" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1050</v>
       </c>
       <c r="H730" s="22">
-        <v>0</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="I730" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J730" t="str">
+        <v>1400</v>
+      </c>
+      <c r="J730">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6123</v>
       </c>
       <c r="K730" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L730" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L730">
         <f t="shared" si="103"/>
-        <v/>
+        <v>1400</v>
       </c>
     </row>
     <row r="731" spans="1:12">
-      <c r="A731" s="15"/>
-      <c r="B731" s="16"/>
+      <c r="A731" s="15">
+        <v>6124</v>
+      </c>
+      <c r="B731" s="16" t="s">
+        <v>678</v>
+      </c>
       <c r="C731" s="17">
         <v>1032</v>
       </c>
@@ -33446,38 +33700,42 @@
         <v>15</v>
       </c>
       <c r="E731" s="57">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="F731" s="20">
         <v>0</v>
       </c>
       <c r="G731" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="H731" s="22">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="I731" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J731" t="str">
+        <v>1650</v>
+      </c>
+      <c r="J731">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6124</v>
       </c>
       <c r="K731" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L731" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L731">
         <f t="shared" si="103"/>
-        <v/>
+        <v>1650</v>
       </c>
     </row>
     <row r="732" spans="1:12">
-      <c r="A732" s="15"/>
-      <c r="B732" s="16"/>
+      <c r="A732" s="15">
+        <v>6125</v>
+      </c>
+      <c r="B732" s="16" t="s">
+        <v>679</v>
+      </c>
       <c r="C732" s="17">
         <v>1032</v>
       </c>
@@ -33485,38 +33743,42 @@
         <v>15</v>
       </c>
       <c r="E732" s="57">
-        <v>0</v>
+        <v>1880</v>
       </c>
       <c r="F732" s="20">
         <v>0</v>
       </c>
       <c r="G732" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1880</v>
       </c>
       <c r="H732" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I732" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J732" t="str">
+        <v>2256</v>
+      </c>
+      <c r="J732">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6125</v>
       </c>
       <c r="K732" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L732" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L732">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2256</v>
       </c>
     </row>
     <row r="733" spans="1:12">
-      <c r="A733" s="15"/>
-      <c r="B733" s="16"/>
+      <c r="A733" s="15">
+        <v>6126</v>
+      </c>
+      <c r="B733" s="16" t="s">
+        <v>680</v>
+      </c>
       <c r="C733" s="17">
         <v>1032</v>
       </c>
@@ -33524,38 +33786,42 @@
         <v>15</v>
       </c>
       <c r="E733" s="57">
-        <v>0</v>
+        <v>1880</v>
       </c>
       <c r="F733" s="20">
         <v>0</v>
       </c>
       <c r="G733" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1880</v>
       </c>
       <c r="H733" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I733" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J733" t="str">
+        <v>2256</v>
+      </c>
+      <c r="J733">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6126</v>
       </c>
       <c r="K733" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L733" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L733">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2256</v>
       </c>
     </row>
     <row r="734" spans="1:12">
-      <c r="A734" s="15"/>
-      <c r="B734" s="16"/>
+      <c r="A734" s="15">
+        <v>6126</v>
+      </c>
+      <c r="B734" s="16" t="s">
+        <v>681</v>
+      </c>
       <c r="C734" s="17">
         <v>1032</v>
       </c>
@@ -33563,38 +33829,42 @@
         <v>15</v>
       </c>
       <c r="E734" s="57">
-        <v>0</v>
+        <v>1880</v>
       </c>
       <c r="F734" s="20">
         <v>0</v>
       </c>
       <c r="G734" s="21">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>1880</v>
       </c>
       <c r="H734" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I734" s="23">
         <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="J734" t="str">
+        <v>2256</v>
+      </c>
+      <c r="J734">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6126</v>
       </c>
       <c r="K734" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L734" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L734">
         <f t="shared" si="103"/>
-        <v/>
+        <v>2256</v>
       </c>
     </row>
     <row r="735" spans="1:12">
-      <c r="A735" s="15"/>
-      <c r="B735" s="16"/>
+      <c r="A735" s="15">
+        <v>6127</v>
+      </c>
+      <c r="B735" s="16" t="s">
+        <v>682</v>
+      </c>
       <c r="C735" s="17">
         <v>1032</v>
       </c>
@@ -33602,38 +33872,42 @@
         <v>15</v>
       </c>
       <c r="E735" s="57">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F735" s="20">
         <v>0</v>
       </c>
       <c r="G735" s="21">
         <f t="shared" ref="G735:G766" si="104">E735*(1-F735)</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="H735" s="22">
         <v>0</v>
       </c>
       <c r="I735" s="23">
         <f t="shared" ref="I735:I766" si="105">+ROUND((G735*H735)+G735,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J735" t="str">
+        <v>3000</v>
+      </c>
+      <c r="J735">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6127</v>
       </c>
       <c r="K735" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L735" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L735">
         <f t="shared" si="103"/>
-        <v/>
+        <v>3000</v>
       </c>
     </row>
     <row r="736" spans="1:12">
-      <c r="A736" s="15"/>
-      <c r="B736" s="16"/>
+      <c r="A736" s="15">
+        <v>6130</v>
+      </c>
+      <c r="B736" s="16" t="s">
+        <v>683</v>
+      </c>
       <c r="C736" s="17">
         <v>1032</v>
       </c>
@@ -33641,33 +33915,33 @@
         <v>15</v>
       </c>
       <c r="E736" s="57">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F736" s="20">
         <v>0</v>
       </c>
       <c r="G736" s="21">
         <f t="shared" si="104"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="H736" s="22">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="I736" s="23">
         <f t="shared" si="105"/>
-        <v>0</v>
-      </c>
-      <c r="J736" t="str">
+        <v>4000</v>
+      </c>
+      <c r="J736">
         <f t="shared" si="101"/>
-        <v/>
+        <v>6130</v>
       </c>
       <c r="K736" t="str">
         <f t="shared" si="102"/>
-        <v/>
-      </c>
-      <c r="L736" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="L736">
         <f t="shared" si="103"/>
-        <v/>
+        <v>4000</v>
       </c>
     </row>
     <row r="737" spans="1:12">
@@ -43981,7 +44255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView topLeftCell="A652" workbookViewId="0">
@@ -44636,7 +44910,7 @@
       </c>
       <c r="C46">
         <f>IF(PRECIOS_DE_VENTA!L49="","",PRECIOS_DE_VENTA!L49)</f>
-        <v>5999</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -44874,7 +45148,7 @@
       </c>
       <c r="C63">
         <f>IF(PRECIOS_DE_VENTA!L66="","",PRECIOS_DE_VENTA!L66)</f>
-        <v>9999</v>
+        <v>9290</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -51454,7 +51728,7 @@
       </c>
       <c r="C533">
         <f>IF(PRECIOS_DE_VENTA!L536="","",PRECIOS_DE_VENTA!L536)</f>
-        <v>13670</v>
+        <v>13290</v>
       </c>
     </row>
     <row r="534" spans="1:3">
@@ -51496,7 +51770,7 @@
       </c>
       <c r="C536">
         <f>IF(PRECIOS_DE_VENTA!L539="","",PRECIOS_DE_VENTA!L539)</f>
-        <v>13068</v>
+        <v>12150</v>
       </c>
     </row>
     <row r="537" spans="1:3">
@@ -51580,7 +51854,7 @@
       </c>
       <c r="C542">
         <f>IF(PRECIOS_DE_VENTA!L545="","",PRECIOS_DE_VENTA!L545)</f>
-        <v>24840</v>
+        <v>12100</v>
       </c>
     </row>
     <row r="543" spans="1:3">
@@ -51958,7 +52232,7 @@
       </c>
       <c r="C569">
         <f>IF(PRECIOS_DE_VENTA!L572="","",PRECIOS_DE_VENTA!L572)</f>
-        <v>14844</v>
+        <v>13669</v>
       </c>
     </row>
     <row r="570" spans="1:3">
@@ -52014,7 +52288,7 @@
       </c>
       <c r="C573">
         <f>IF(PRECIOS_DE_VENTA!L576="","",PRECIOS_DE_VENTA!L576)</f>
-        <v>7608</v>
+        <v>7620</v>
       </c>
     </row>
     <row r="574" spans="1:3">
@@ -52042,7 +52316,7 @@
       </c>
       <c r="C575">
         <f>IF(PRECIOS_DE_VENTA!L578="","",PRECIOS_DE_VENTA!L578)</f>
-        <v>7841</v>
+        <v>7300</v>
       </c>
     </row>
     <row r="576" spans="1:3">
@@ -52056,7 +52330,7 @@
       </c>
       <c r="C576">
         <f>IF(PRECIOS_DE_VENTA!L579="","",PRECIOS_DE_VENTA!L579)</f>
-        <v>8474</v>
+        <v>7299</v>
       </c>
     </row>
     <row r="577" spans="1:3">
@@ -52070,7 +52344,7 @@
       </c>
       <c r="C577">
         <f>IF(PRECIOS_DE_VENTA!L580="","",PRECIOS_DE_VENTA!L580)</f>
-        <v>8152</v>
+        <v>8787</v>
       </c>
     </row>
     <row r="578" spans="1:3">
@@ -52084,7 +52358,7 @@
       </c>
       <c r="C578">
         <f>IF(PRECIOS_DE_VENTA!L581="","",PRECIOS_DE_VENTA!L581)</f>
-        <v>6615</v>
+        <v>6620</v>
       </c>
     </row>
     <row r="579" spans="1:3">
@@ -52112,7 +52386,7 @@
       </c>
       <c r="C580">
         <f>IF(PRECIOS_DE_VENTA!L583="","",PRECIOS_DE_VENTA!L583)</f>
-        <v>8676</v>
+        <v>7899</v>
       </c>
     </row>
     <row r="581" spans="1:3">
@@ -52126,7 +52400,7 @@
       </c>
       <c r="C581">
         <f>IF(PRECIOS_DE_VENTA!L584="","",PRECIOS_DE_VENTA!L584)</f>
-        <v>14813</v>
+        <v>14799</v>
       </c>
     </row>
     <row r="582" spans="1:3">
@@ -52140,7 +52414,7 @@
       </c>
       <c r="C582">
         <f>IF(PRECIOS_DE_VENTA!L585="","",PRECIOS_DE_VENTA!L585)</f>
-        <v>7500</v>
+        <v>8300</v>
       </c>
     </row>
     <row r="583" spans="1:3">
@@ -52252,7 +52526,7 @@
       </c>
       <c r="C590">
         <f>IF(PRECIOS_DE_VENTA!L593="","",PRECIOS_DE_VENTA!L593)</f>
-        <v>8643</v>
+        <v>8649</v>
       </c>
     </row>
     <row r="591" spans="1:3">
@@ -52280,7 +52554,7 @@
       </c>
       <c r="C592">
         <f>IF(PRECIOS_DE_VENTA!L595="","",PRECIOS_DE_VENTA!L595)</f>
-        <v>10936</v>
+        <v>10940</v>
       </c>
     </row>
     <row r="593" spans="1:3">
@@ -52294,7 +52568,7 @@
       </c>
       <c r="C593">
         <f>IF(PRECIOS_DE_VENTA!L596="","",PRECIOS_DE_VENTA!L596)</f>
-        <v>8641</v>
+        <v>8650</v>
       </c>
     </row>
     <row r="594" spans="1:3">
@@ -52308,7 +52582,7 @@
       </c>
       <c r="C594">
         <f>IF(PRECIOS_DE_VENTA!L597="","",PRECIOS_DE_VENTA!L597)</f>
-        <v>8641</v>
+        <v>7499</v>
       </c>
     </row>
     <row r="595" spans="1:3">
@@ -52322,7 +52596,7 @@
       </c>
       <c r="C595">
         <f>IF(PRECIOS_DE_VENTA!L598="","",PRECIOS_DE_VENTA!L598)</f>
-        <v>8455</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="596" spans="1:3">
@@ -52350,7 +52624,7 @@
       </c>
       <c r="C597">
         <f>IF(PRECIOS_DE_VENTA!L600="","",PRECIOS_DE_VENTA!L600)</f>
-        <v>6999</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="598" spans="1:3">
@@ -52378,7 +52652,7 @@
       </c>
       <c r="C599">
         <f>IF(PRECIOS_DE_VENTA!L602="","",PRECIOS_DE_VENTA!L602)</f>
-        <v>9236</v>
+        <v>9240</v>
       </c>
     </row>
     <row r="600" spans="1:3">
@@ -52490,7 +52764,7 @@
       </c>
       <c r="C607">
         <f>IF(PRECIOS_DE_VENTA!L610="","",PRECIOS_DE_VENTA!L610)</f>
-        <v>1400</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="608" spans="1:3">
@@ -52532,7 +52806,7 @@
       </c>
       <c r="C610">
         <f>IF(PRECIOS_DE_VENTA!L613="","",PRECIOS_DE_VENTA!L613)</f>
-        <v>1800</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="611" spans="1:3">
@@ -52588,7 +52862,7 @@
       </c>
       <c r="C614">
         <f>IF(PRECIOS_DE_VENTA!L617="","",PRECIOS_DE_VENTA!L617)</f>
-        <v>2799</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="615" spans="1:3">
@@ -53036,7 +53310,7 @@
       </c>
       <c r="C646">
         <f>IF(PRECIOS_DE_VENTA!L649="","",PRECIOS_DE_VENTA!L649)</f>
-        <v>2400</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="647" spans="1:3">
@@ -53330,7 +53604,7 @@
       </c>
       <c r="C667">
         <f>IF(PRECIOS_DE_VENTA!L670="","",PRECIOS_DE_VENTA!L670)</f>
-        <v>4200</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="668" spans="1:3">
@@ -53386,7 +53660,7 @@
       </c>
       <c r="C671">
         <f>IF(PRECIOS_DE_VENTA!L674="","",PRECIOS_DE_VENTA!L674)</f>
-        <v>6500</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="672" spans="1:3">
@@ -53400,7 +53674,7 @@
       </c>
       <c r="C672">
         <f>IF(PRECIOS_DE_VENTA!L675="","",PRECIOS_DE_VENTA!L675)</f>
-        <v>2500</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="673" spans="1:3">
@@ -53554,7 +53828,7 @@
       </c>
       <c r="C683">
         <f>IF(PRECIOS_DE_VENTA!L686="","",PRECIOS_DE_VENTA!L686)</f>
-        <v>1855</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="684" spans="1:3">
@@ -53568,7 +53842,7 @@
       </c>
       <c r="C684">
         <f>IF(PRECIOS_DE_VENTA!L687="","",PRECIOS_DE_VENTA!L687)</f>
-        <v>10400</v>
+        <v>11050</v>
       </c>
     </row>
     <row r="685" spans="1:3">
@@ -53624,7 +53898,7 @@
       </c>
       <c r="C688">
         <f>IF(PRECIOS_DE_VENTA!L691="","",PRECIOS_DE_VENTA!L691)</f>
-        <v>2600</v>
+        <v>100</v>
       </c>
     </row>
     <row r="689" spans="1:3">
@@ -53708,553 +53982,553 @@
       </c>
       <c r="C694">
         <f>IF(PRECIOS_DE_VENTA!L697="","",PRECIOS_DE_VENTA!L697)</f>
-        <v>3700</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="695" spans="1:3">
-      <c r="A695" t="str">
+      <c r="A695">
         <f>IF(PRECIOS_DE_VENTA!J698="","",PRECIOS_DE_VENTA!J698)</f>
-        <v/>
+        <v>999</v>
       </c>
       <c r="B695" t="str">
         <f>IF(PRECIOS_DE_VENTA!K698="","",PRECIOS_DE_VENTA!K698)</f>
-        <v/>
-      </c>
-      <c r="C695" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C695">
         <f>IF(PRECIOS_DE_VENTA!L698="","",PRECIOS_DE_VENTA!L698)</f>
-        <v/>
+        <v>7000</v>
       </c>
     </row>
     <row r="696" spans="1:3">
-      <c r="A696" t="str">
+      <c r="A696">
         <f>IF(PRECIOS_DE_VENTA!J699="","",PRECIOS_DE_VENTA!J699)</f>
-        <v/>
+        <v>6091</v>
       </c>
       <c r="B696" t="str">
         <f>IF(PRECIOS_DE_VENTA!K699="","",PRECIOS_DE_VENTA!K699)</f>
-        <v/>
-      </c>
-      <c r="C696" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C696">
         <f>IF(PRECIOS_DE_VENTA!L699="","",PRECIOS_DE_VENTA!L699)</f>
-        <v/>
+        <v>2390</v>
       </c>
     </row>
     <row r="697" spans="1:3">
-      <c r="A697" t="str">
+      <c r="A697">
         <f>IF(PRECIOS_DE_VENTA!J700="","",PRECIOS_DE_VENTA!J700)</f>
-        <v/>
+        <v>6092</v>
       </c>
       <c r="B697" t="str">
         <f>IF(PRECIOS_DE_VENTA!K700="","",PRECIOS_DE_VENTA!K700)</f>
-        <v/>
-      </c>
-      <c r="C697" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C697">
         <f>IF(PRECIOS_DE_VENTA!L700="","",PRECIOS_DE_VENTA!L700)</f>
-        <v/>
+        <v>3489</v>
       </c>
     </row>
     <row r="698" spans="1:3">
-      <c r="A698" t="str">
+      <c r="A698">
         <f>IF(PRECIOS_DE_VENTA!J701="","",PRECIOS_DE_VENTA!J701)</f>
-        <v/>
+        <v>6093</v>
       </c>
       <c r="B698" t="str">
         <f>IF(PRECIOS_DE_VENTA!K701="","",PRECIOS_DE_VENTA!K701)</f>
-        <v/>
-      </c>
-      <c r="C698" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C698">
         <f>IF(PRECIOS_DE_VENTA!L701="","",PRECIOS_DE_VENTA!L701)</f>
-        <v/>
+        <v>2600</v>
       </c>
     </row>
     <row r="699" spans="1:3">
-      <c r="A699" t="str">
+      <c r="A699">
         <f>IF(PRECIOS_DE_VENTA!J702="","",PRECIOS_DE_VENTA!J702)</f>
-        <v/>
+        <v>6094</v>
       </c>
       <c r="B699" t="str">
         <f>IF(PRECIOS_DE_VENTA!K702="","",PRECIOS_DE_VENTA!K702)</f>
-        <v/>
-      </c>
-      <c r="C699" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C699">
         <f>IF(PRECIOS_DE_VENTA!L702="","",PRECIOS_DE_VENTA!L702)</f>
-        <v/>
+        <v>3094</v>
       </c>
     </row>
     <row r="700" spans="1:3">
-      <c r="A700" t="str">
+      <c r="A700">
         <f>IF(PRECIOS_DE_VENTA!J703="","",PRECIOS_DE_VENTA!J703)</f>
-        <v/>
+        <v>6095</v>
       </c>
       <c r="B700" t="str">
         <f>IF(PRECIOS_DE_VENTA!K703="","",PRECIOS_DE_VENTA!K703)</f>
-        <v/>
-      </c>
-      <c r="C700" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C700">
         <f>IF(PRECIOS_DE_VENTA!L703="","",PRECIOS_DE_VENTA!L703)</f>
-        <v/>
+        <v>1755</v>
       </c>
     </row>
     <row r="701" spans="1:3">
-      <c r="A701" t="str">
+      <c r="A701">
         <f>IF(PRECIOS_DE_VENTA!J704="","",PRECIOS_DE_VENTA!J704)</f>
-        <v/>
+        <v>6096</v>
       </c>
       <c r="B701" t="str">
         <f>IF(PRECIOS_DE_VENTA!K704="","",PRECIOS_DE_VENTA!K704)</f>
-        <v/>
-      </c>
-      <c r="C701" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C701">
         <f>IF(PRECIOS_DE_VENTA!L704="","",PRECIOS_DE_VENTA!L704)</f>
-        <v/>
+        <v>8099</v>
       </c>
     </row>
     <row r="702" spans="1:3">
-      <c r="A702" t="str">
+      <c r="A702">
         <f>IF(PRECIOS_DE_VENTA!J705="","",PRECIOS_DE_VENTA!J705)</f>
-        <v/>
+        <v>6097</v>
       </c>
       <c r="B702" t="str">
         <f>IF(PRECIOS_DE_VENTA!K705="","",PRECIOS_DE_VENTA!K705)</f>
-        <v/>
-      </c>
-      <c r="C702" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C702">
         <f>IF(PRECIOS_DE_VENTA!L705="","",PRECIOS_DE_VENTA!L705)</f>
-        <v/>
+        <v>7800</v>
       </c>
     </row>
     <row r="703" spans="1:3">
-      <c r="A703" t="str">
+      <c r="A703">
         <f>IF(PRECIOS_DE_VENTA!J706="","",PRECIOS_DE_VENTA!J706)</f>
-        <v/>
+        <v>6098</v>
       </c>
       <c r="B703" t="str">
         <f>IF(PRECIOS_DE_VENTA!K706="","",PRECIOS_DE_VENTA!K706)</f>
-        <v/>
-      </c>
-      <c r="C703" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C703">
         <f>IF(PRECIOS_DE_VENTA!L706="","",PRECIOS_DE_VENTA!L706)</f>
-        <v/>
+        <v>850</v>
       </c>
     </row>
     <row r="704" spans="1:3">
-      <c r="A704" t="str">
+      <c r="A704">
         <f>IF(PRECIOS_DE_VENTA!J707="","",PRECIOS_DE_VENTA!J707)</f>
-        <v/>
+        <v>6099</v>
       </c>
       <c r="B704" t="str">
         <f>IF(PRECIOS_DE_VENTA!K707="","",PRECIOS_DE_VENTA!K707)</f>
-        <v/>
-      </c>
-      <c r="C704" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C704">
         <f>IF(PRECIOS_DE_VENTA!L707="","",PRECIOS_DE_VENTA!L707)</f>
-        <v/>
+        <v>4123</v>
       </c>
     </row>
     <row r="705" spans="1:3">
-      <c r="A705" t="str">
+      <c r="A705">
         <f>IF(PRECIOS_DE_VENTA!J708="","",PRECIOS_DE_VENTA!J708)</f>
-        <v/>
+        <v>6100</v>
       </c>
       <c r="B705" t="str">
         <f>IF(PRECIOS_DE_VENTA!K708="","",PRECIOS_DE_VENTA!K708)</f>
-        <v/>
-      </c>
-      <c r="C705" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C705">
         <f>IF(PRECIOS_DE_VENTA!L708="","",PRECIOS_DE_VENTA!L708)</f>
-        <v/>
+        <v>1550</v>
       </c>
     </row>
     <row r="706" spans="1:3">
-      <c r="A706" t="str">
+      <c r="A706">
         <f>IF(PRECIOS_DE_VENTA!J709="","",PRECIOS_DE_VENTA!J709)</f>
-        <v/>
+        <v>6101</v>
       </c>
       <c r="B706" t="str">
         <f>IF(PRECIOS_DE_VENTA!K709="","",PRECIOS_DE_VENTA!K709)</f>
-        <v/>
-      </c>
-      <c r="C706" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C706">
         <f>IF(PRECIOS_DE_VENTA!L709="","",PRECIOS_DE_VENTA!L709)</f>
-        <v/>
+        <v>6159</v>
       </c>
     </row>
     <row r="707" spans="1:3">
-      <c r="A707" t="str">
+      <c r="A707">
         <f>IF(PRECIOS_DE_VENTA!J710="","",PRECIOS_DE_VENTA!J710)</f>
-        <v/>
+        <v>6102</v>
       </c>
       <c r="B707" t="str">
         <f>IF(PRECIOS_DE_VENTA!K710="","",PRECIOS_DE_VENTA!K710)</f>
-        <v/>
-      </c>
-      <c r="C707" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C707">
         <f>IF(PRECIOS_DE_VENTA!L710="","",PRECIOS_DE_VENTA!L710)</f>
-        <v/>
+        <v>3300</v>
       </c>
     </row>
     <row r="708" spans="1:3">
-      <c r="A708" t="str">
+      <c r="A708">
         <f>IF(PRECIOS_DE_VENTA!J711="","",PRECIOS_DE_VENTA!J711)</f>
-        <v/>
+        <v>6103</v>
       </c>
       <c r="B708" t="str">
         <f>IF(PRECIOS_DE_VENTA!K711="","",PRECIOS_DE_VENTA!K711)</f>
-        <v/>
-      </c>
-      <c r="C708" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C708">
         <f>IF(PRECIOS_DE_VENTA!L711="","",PRECIOS_DE_VENTA!L711)</f>
-        <v/>
+        <v>2500</v>
       </c>
     </row>
     <row r="709" spans="1:3">
-      <c r="A709" t="str">
+      <c r="A709">
         <f>IF(PRECIOS_DE_VENTA!J712="","",PRECIOS_DE_VENTA!J712)</f>
-        <v/>
+        <v>6104</v>
       </c>
       <c r="B709" t="str">
         <f>IF(PRECIOS_DE_VENTA!K712="","",PRECIOS_DE_VENTA!K712)</f>
-        <v/>
-      </c>
-      <c r="C709" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C709">
         <f>IF(PRECIOS_DE_VENTA!L712="","",PRECIOS_DE_VENTA!L712)</f>
-        <v/>
+        <v>1325</v>
       </c>
     </row>
     <row r="710" spans="1:3">
-      <c r="A710" t="str">
+      <c r="A710">
         <f>IF(PRECIOS_DE_VENTA!J713="","",PRECIOS_DE_VENTA!J713)</f>
-        <v/>
+        <v>6105</v>
       </c>
       <c r="B710" t="str">
         <f>IF(PRECIOS_DE_VENTA!K713="","",PRECIOS_DE_VENTA!K713)</f>
-        <v/>
-      </c>
-      <c r="C710" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C710">
         <f>IF(PRECIOS_DE_VENTA!L713="","",PRECIOS_DE_VENTA!L713)</f>
-        <v/>
+        <v>2210</v>
       </c>
     </row>
     <row r="711" spans="1:3">
-      <c r="A711" t="str">
+      <c r="A711">
         <f>IF(PRECIOS_DE_VENTA!J714="","",PRECIOS_DE_VENTA!J714)</f>
-        <v/>
+        <v>6106</v>
       </c>
       <c r="B711" t="str">
         <f>IF(PRECIOS_DE_VENTA!K714="","",PRECIOS_DE_VENTA!K714)</f>
-        <v/>
-      </c>
-      <c r="C711" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C711">
         <f>IF(PRECIOS_DE_VENTA!L714="","",PRECIOS_DE_VENTA!L714)</f>
-        <v/>
+        <v>2730</v>
       </c>
     </row>
     <row r="712" spans="1:3">
-      <c r="A712" t="str">
+      <c r="A712">
         <f>IF(PRECIOS_DE_VENTA!J715="","",PRECIOS_DE_VENTA!J715)</f>
-        <v/>
+        <v>6107</v>
       </c>
       <c r="B712" t="str">
         <f>IF(PRECIOS_DE_VENTA!K715="","",PRECIOS_DE_VENTA!K715)</f>
-        <v/>
-      </c>
-      <c r="C712" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C712">
         <f>IF(PRECIOS_DE_VENTA!L715="","",PRECIOS_DE_VENTA!L715)</f>
-        <v/>
+        <v>2730</v>
       </c>
     </row>
     <row r="713" spans="1:3">
-      <c r="A713" t="str">
+      <c r="A713">
         <f>IF(PRECIOS_DE_VENTA!J716="","",PRECIOS_DE_VENTA!J716)</f>
-        <v/>
+        <v>6108</v>
       </c>
       <c r="B713" t="str">
         <f>IF(PRECIOS_DE_VENTA!K716="","",PRECIOS_DE_VENTA!K716)</f>
-        <v/>
-      </c>
-      <c r="C713" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C713">
         <f>IF(PRECIOS_DE_VENTA!L716="","",PRECIOS_DE_VENTA!L716)</f>
-        <v/>
+        <v>2730</v>
       </c>
     </row>
     <row r="714" spans="1:3">
-      <c r="A714" t="str">
+      <c r="A714">
         <f>IF(PRECIOS_DE_VENTA!J717="","",PRECIOS_DE_VENTA!J717)</f>
-        <v/>
+        <v>6109</v>
       </c>
       <c r="B714" t="str">
         <f>IF(PRECIOS_DE_VENTA!K717="","",PRECIOS_DE_VENTA!K717)</f>
-        <v/>
-      </c>
-      <c r="C714" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C714">
         <f>IF(PRECIOS_DE_VENTA!L717="","",PRECIOS_DE_VENTA!L717)</f>
-        <v/>
+        <v>8220</v>
       </c>
     </row>
     <row r="715" spans="1:3">
-      <c r="A715" t="str">
+      <c r="A715">
         <f>IF(PRECIOS_DE_VENTA!J718="","",PRECIOS_DE_VENTA!J718)</f>
-        <v/>
+        <v>6110</v>
       </c>
       <c r="B715" t="str">
         <f>IF(PRECIOS_DE_VENTA!K718="","",PRECIOS_DE_VENTA!K718)</f>
-        <v/>
-      </c>
-      <c r="C715" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C715">
         <f>IF(PRECIOS_DE_VENTA!L718="","",PRECIOS_DE_VENTA!L718)</f>
-        <v/>
+        <v>2259</v>
       </c>
     </row>
     <row r="716" spans="1:3">
-      <c r="A716" t="str">
+      <c r="A716">
         <f>IF(PRECIOS_DE_VENTA!J719="","",PRECIOS_DE_VENTA!J719)</f>
-        <v/>
+        <v>6111</v>
       </c>
       <c r="B716" t="str">
         <f>IF(PRECIOS_DE_VENTA!K719="","",PRECIOS_DE_VENTA!K719)</f>
-        <v/>
-      </c>
-      <c r="C716" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C716">
         <f>IF(PRECIOS_DE_VENTA!L719="","",PRECIOS_DE_VENTA!L719)</f>
-        <v/>
+        <v>2550</v>
       </c>
     </row>
     <row r="717" spans="1:3">
-      <c r="A717" t="str">
+      <c r="A717">
         <f>IF(PRECIOS_DE_VENTA!J720="","",PRECIOS_DE_VENTA!J720)</f>
-        <v/>
+        <v>6112</v>
       </c>
       <c r="B717" t="str">
         <f>IF(PRECIOS_DE_VENTA!K720="","",PRECIOS_DE_VENTA!K720)</f>
-        <v/>
-      </c>
-      <c r="C717" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C717">
         <f>IF(PRECIOS_DE_VENTA!L720="","",PRECIOS_DE_VENTA!L720)</f>
-        <v/>
+        <v>1204</v>
       </c>
     </row>
     <row r="718" spans="1:3">
-      <c r="A718" t="str">
+      <c r="A718">
         <f>IF(PRECIOS_DE_VENTA!J721="","",PRECIOS_DE_VENTA!J721)</f>
-        <v/>
+        <v>6113</v>
       </c>
       <c r="B718" t="str">
         <f>IF(PRECIOS_DE_VENTA!K721="","",PRECIOS_DE_VENTA!K721)</f>
-        <v/>
-      </c>
-      <c r="C718" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C718">
         <f>IF(PRECIOS_DE_VENTA!L721="","",PRECIOS_DE_VENTA!L721)</f>
-        <v/>
+        <v>1150</v>
       </c>
     </row>
     <row r="719" spans="1:3">
-      <c r="A719" t="str">
+      <c r="A719">
         <f>IF(PRECIOS_DE_VENTA!J722="","",PRECIOS_DE_VENTA!J722)</f>
-        <v/>
+        <v>6114</v>
       </c>
       <c r="B719" t="str">
         <f>IF(PRECIOS_DE_VENTA!K722="","",PRECIOS_DE_VENTA!K722)</f>
-        <v/>
-      </c>
-      <c r="C719" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C719">
         <f>IF(PRECIOS_DE_VENTA!L722="","",PRECIOS_DE_VENTA!L722)</f>
-        <v/>
+        <v>3199</v>
       </c>
     </row>
     <row r="720" spans="1:3">
-      <c r="A720" t="str">
+      <c r="A720">
         <f>IF(PRECIOS_DE_VENTA!J723="","",PRECIOS_DE_VENTA!J723)</f>
-        <v/>
+        <v>6115</v>
       </c>
       <c r="B720" t="str">
         <f>IF(PRECIOS_DE_VENTA!K723="","",PRECIOS_DE_VENTA!K723)</f>
-        <v/>
-      </c>
-      <c r="C720" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C720">
         <f>IF(PRECIOS_DE_VENTA!L723="","",PRECIOS_DE_VENTA!L723)</f>
-        <v/>
+        <v>2380</v>
       </c>
     </row>
     <row r="721" spans="1:3">
-      <c r="A721" t="str">
+      <c r="A721">
         <f>IF(PRECIOS_DE_VENTA!J724="","",PRECIOS_DE_VENTA!J724)</f>
-        <v/>
+        <v>6116</v>
       </c>
       <c r="B721" t="str">
         <f>IF(PRECIOS_DE_VENTA!K724="","",PRECIOS_DE_VENTA!K724)</f>
-        <v/>
-      </c>
-      <c r="C721" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C721">
         <f>IF(PRECIOS_DE_VENTA!L724="","",PRECIOS_DE_VENTA!L724)</f>
-        <v/>
+        <v>4399</v>
       </c>
     </row>
     <row r="722" spans="1:3">
-      <c r="A722" t="str">
+      <c r="A722">
         <f>IF(PRECIOS_DE_VENTA!J725="","",PRECIOS_DE_VENTA!J725)</f>
-        <v/>
+        <v>6117</v>
       </c>
       <c r="B722" t="str">
         <f>IF(PRECIOS_DE_VENTA!K725="","",PRECIOS_DE_VENTA!K725)</f>
-        <v/>
-      </c>
-      <c r="C722" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C722">
         <f>IF(PRECIOS_DE_VENTA!L725="","",PRECIOS_DE_VENTA!L725)</f>
-        <v/>
+        <v>2600</v>
       </c>
     </row>
     <row r="723" spans="1:3">
-      <c r="A723" t="str">
+      <c r="A723">
         <f>IF(PRECIOS_DE_VENTA!J726="","",PRECIOS_DE_VENTA!J726)</f>
-        <v/>
+        <v>6118</v>
       </c>
       <c r="B723" t="str">
         <f>IF(PRECIOS_DE_VENTA!K726="","",PRECIOS_DE_VENTA!K726)</f>
-        <v/>
-      </c>
-      <c r="C723" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C723">
         <f>IF(PRECIOS_DE_VENTA!L726="","",PRECIOS_DE_VENTA!L726)</f>
-        <v/>
+        <v>8890</v>
       </c>
     </row>
     <row r="724" spans="1:3">
-      <c r="A724" t="str">
+      <c r="A724">
         <f>IF(PRECIOS_DE_VENTA!J727="","",PRECIOS_DE_VENTA!J727)</f>
-        <v/>
+        <v>6120</v>
       </c>
       <c r="B724" t="str">
         <f>IF(PRECIOS_DE_VENTA!K727="","",PRECIOS_DE_VENTA!K727)</f>
-        <v/>
-      </c>
-      <c r="C724" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C724">
         <f>IF(PRECIOS_DE_VENTA!L727="","",PRECIOS_DE_VENTA!L727)</f>
-        <v/>
+        <v>1760</v>
       </c>
     </row>
     <row r="725" spans="1:3">
-      <c r="A725" t="str">
+      <c r="A725">
         <f>IF(PRECIOS_DE_VENTA!J728="","",PRECIOS_DE_VENTA!J728)</f>
-        <v/>
+        <v>6121</v>
       </c>
       <c r="B725" t="str">
         <f>IF(PRECIOS_DE_VENTA!K728="","",PRECIOS_DE_VENTA!K728)</f>
-        <v/>
-      </c>
-      <c r="C725" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C725">
         <f>IF(PRECIOS_DE_VENTA!L728="","",PRECIOS_DE_VENTA!L728)</f>
-        <v/>
+        <v>1470</v>
       </c>
     </row>
     <row r="726" spans="1:3">
-      <c r="A726" t="str">
+      <c r="A726">
         <f>IF(PRECIOS_DE_VENTA!J729="","",PRECIOS_DE_VENTA!J729)</f>
-        <v/>
+        <v>6122</v>
       </c>
       <c r="B726" t="str">
         <f>IF(PRECIOS_DE_VENTA!K729="","",PRECIOS_DE_VENTA!K729)</f>
-        <v/>
-      </c>
-      <c r="C726" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C726">
         <f>IF(PRECIOS_DE_VENTA!L729="","",PRECIOS_DE_VENTA!L729)</f>
-        <v/>
+        <v>1400</v>
       </c>
     </row>
     <row r="727" spans="1:3">
-      <c r="A727" t="str">
+      <c r="A727">
         <f>IF(PRECIOS_DE_VENTA!J730="","",PRECIOS_DE_VENTA!J730)</f>
-        <v/>
+        <v>6123</v>
       </c>
       <c r="B727" t="str">
         <f>IF(PRECIOS_DE_VENTA!K730="","",PRECIOS_DE_VENTA!K730)</f>
-        <v/>
-      </c>
-      <c r="C727" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C727">
         <f>IF(PRECIOS_DE_VENTA!L730="","",PRECIOS_DE_VENTA!L730)</f>
-        <v/>
+        <v>1400</v>
       </c>
     </row>
     <row r="728" spans="1:3">
-      <c r="A728" t="str">
+      <c r="A728">
         <f>IF(PRECIOS_DE_VENTA!J731="","",PRECIOS_DE_VENTA!J731)</f>
-        <v/>
+        <v>6124</v>
       </c>
       <c r="B728" t="str">
         <f>IF(PRECIOS_DE_VENTA!K731="","",PRECIOS_DE_VENTA!K731)</f>
-        <v/>
-      </c>
-      <c r="C728" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C728">
         <f>IF(PRECIOS_DE_VENTA!L731="","",PRECIOS_DE_VENTA!L731)</f>
-        <v/>
+        <v>1650</v>
       </c>
     </row>
     <row r="729" spans="1:3">
-      <c r="A729" t="str">
+      <c r="A729">
         <f>IF(PRECIOS_DE_VENTA!J732="","",PRECIOS_DE_VENTA!J732)</f>
-        <v/>
+        <v>6125</v>
       </c>
       <c r="B729" t="str">
         <f>IF(PRECIOS_DE_VENTA!K732="","",PRECIOS_DE_VENTA!K732)</f>
-        <v/>
-      </c>
-      <c r="C729" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C729">
         <f>IF(PRECIOS_DE_VENTA!L732="","",PRECIOS_DE_VENTA!L732)</f>
-        <v/>
+        <v>2256</v>
       </c>
     </row>
     <row r="730" spans="1:3">
-      <c r="A730" t="str">
+      <c r="A730">
         <f>IF(PRECIOS_DE_VENTA!J733="","",PRECIOS_DE_VENTA!J733)</f>
-        <v/>
+        <v>6126</v>
       </c>
       <c r="B730" t="str">
         <f>IF(PRECIOS_DE_VENTA!K733="","",PRECIOS_DE_VENTA!K733)</f>
-        <v/>
-      </c>
-      <c r="C730" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C730">
         <f>IF(PRECIOS_DE_VENTA!L733="","",PRECIOS_DE_VENTA!L733)</f>
-        <v/>
+        <v>2256</v>
       </c>
     </row>
     <row r="731" spans="1:3">
-      <c r="A731" t="str">
+      <c r="A731">
         <f>IF(PRECIOS_DE_VENTA!J734="","",PRECIOS_DE_VENTA!J734)</f>
-        <v/>
+        <v>6126</v>
       </c>
       <c r="B731" t="str">
         <f>IF(PRECIOS_DE_VENTA!K734="","",PRECIOS_DE_VENTA!K734)</f>
-        <v/>
-      </c>
-      <c r="C731" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C731">
         <f>IF(PRECIOS_DE_VENTA!L734="","",PRECIOS_DE_VENTA!L734)</f>
-        <v/>
+        <v>2256</v>
       </c>
     </row>
     <row r="732" spans="1:3">
-      <c r="A732" t="str">
+      <c r="A732">
         <f>IF(PRECIOS_DE_VENTA!J735="","",PRECIOS_DE_VENTA!J735)</f>
-        <v/>
+        <v>6127</v>
       </c>
       <c r="B732" t="str">
         <f>IF(PRECIOS_DE_VENTA!K735="","",PRECIOS_DE_VENTA!K735)</f>
-        <v/>
-      </c>
-      <c r="C732" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C732">
         <f>IF(PRECIOS_DE_VENTA!L735="","",PRECIOS_DE_VENTA!L735)</f>
-        <v/>
+        <v>3000</v>
       </c>
     </row>
     <row r="733" spans="1:3">
-      <c r="A733" t="str">
+      <c r="A733">
         <f>IF(PRECIOS_DE_VENTA!J736="","",PRECIOS_DE_VENTA!J736)</f>
-        <v/>
+        <v>6130</v>
       </c>
       <c r="B733" t="str">
         <f>IF(PRECIOS_DE_VENTA!K736="","",PRECIOS_DE_VENTA!K736)</f>
-        <v/>
-      </c>
-      <c r="C733" t="str">
+        <v>LISTA1</v>
+      </c>
+      <c r="C733">
         <f>IF(PRECIOS_DE_VENTA!L736="","",PRECIOS_DE_VENTA!L736)</f>
-        <v/>
+        <v>4000</v>
       </c>
     </row>
     <row r="734" spans="1:3">

</xml_diff>